<commit_message>
Adjustments and clean up to parameters flat files
</commit_message>
<xml_diff>
--- a/inst/extdata/plot_thematic.xlsx
+++ b/inst/extdata/plot_thematic.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenjitomari/Documents/GitHub/cdrs/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00035F87-256A-A147-BBAE-8F1B5E4444CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8927CEDE-4539-F34E-87AD-2C15BE97864A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="740" windowWidth="19520" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="740" windowWidth="19520" windowHeight="17260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="labels" sheetId="2" r:id="rId1"/>
     <sheet name="logic" sheetId="3" r:id="rId2"/>
+    <sheet name="palettes" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="240">
   <si>
     <t>short_label</t>
   </si>
@@ -687,61 +688,73 @@
     <t>supplemental_caption</t>
   </si>
   <si>
-    <t>regex</t>
-  </si>
-  <si>
     <t>plot_type1</t>
   </si>
   <si>
-    <t>plot_type2</t>
-  </si>
-  <si>
     <t>affirmative_level</t>
   </si>
   <si>
-    <t>uncertainty_level</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
-    <t>Q3\_\d$</t>
-  </si>
-  <si>
     <t>dichotomous</t>
   </si>
   <si>
-    <t>categorical</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>Q1\_\d$</t>
-  </si>
-  <si>
-    <t>Q4\_\d$</t>
-  </si>
-  <si>
-    <t>&lt;I Dont know why the Delta is important&gt;</t>
-  </si>
-  <si>
-    <t>Q6\_\d$</t>
-  </si>
-  <si>
-    <t>Q7\_\d{1,2}$</t>
-  </si>
-  <si>
-    <t>Q8\_\d$</t>
-  </si>
-  <si>
-    <t>Q17\_\d$</t>
-  </si>
-  <si>
-    <t>Q24\_\d{1,2}$</t>
-  </si>
-  <si>
     <t>Activities in the Delta</t>
+  </si>
+  <si>
+    <t>pal_id</t>
+  </si>
+  <si>
+    <t>plot_type</t>
+  </si>
+  <si>
+    <t>pal_fun</t>
+  </si>
+  <si>
+    <t>pal_name</t>
+  </si>
+  <si>
+    <t>pal_start</t>
+  </si>
+  <si>
+    <t>pal_diff</t>
+  </si>
+  <si>
+    <t>pal_options</t>
+  </si>
+  <si>
+    <t>grDevices::hcl.colors</t>
+  </si>
+  <si>
+    <t>BluYl</t>
+  </si>
+  <si>
+    <t>purples1</t>
+  </si>
+  <si>
+    <t>Magenta</t>
+  </si>
+  <si>
+    <t>mint2</t>
+  </si>
+  <si>
+    <t>Dark Mint</t>
+  </si>
+  <si>
+    <t>mako3</t>
+  </si>
+  <si>
+    <t>Mako</t>
+  </si>
+  <si>
+    <t>blues3</t>
+  </si>
+  <si>
+    <t>Blues 3</t>
   </si>
 </sst>
 </file>
@@ -1604,8 +1617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2543,7 +2556,7 @@
         <v>84</v>
       </c>
       <c r="B41" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="C41" t="s">
         <v>183</v>
@@ -2566,7 +2579,7 @@
         <v>85</v>
       </c>
       <c r="B42" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="C42" t="s">
         <v>184</v>
@@ -2589,7 +2602,7 @@
         <v>87</v>
       </c>
       <c r="B43" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="C43" t="s">
         <v>185</v>
@@ -2612,7 +2625,7 @@
         <v>89</v>
       </c>
       <c r="B44" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="C44" t="s">
         <v>186</v>
@@ -2635,7 +2648,7 @@
         <v>91</v>
       </c>
       <c r="B45" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="C45" t="s">
         <v>187</v>
@@ -2658,7 +2671,7 @@
         <v>93</v>
       </c>
       <c r="B46" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="C46" t="s">
         <v>188</v>
@@ -2681,7 +2694,7 @@
         <v>95</v>
       </c>
       <c r="B47" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="C47" t="s">
         <v>189</v>
@@ -3304,1698 +3317,1162 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="30.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="5" max="5" width="31.6640625" customWidth="1"/>
-    <col min="6" max="6" width="56.83203125" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="4" max="4" width="31.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>220</v>
+      </c>
+      <c r="C4" t="s">
+        <v>232</v>
+      </c>
+      <c r="D4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C5" t="s">
+        <v>232</v>
+      </c>
+      <c r="D5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C6" t="s">
+        <v>232</v>
+      </c>
+      <c r="D6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>220</v>
+      </c>
+      <c r="C7" t="s">
+        <v>232</v>
+      </c>
+      <c r="D7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>220</v>
+      </c>
+      <c r="C8" t="s">
+        <v>232</v>
+      </c>
+      <c r="D8" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C9" t="s">
+        <v>232</v>
+      </c>
+      <c r="D9" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>220</v>
+      </c>
+      <c r="C10" t="s">
+        <v>232</v>
+      </c>
+      <c r="D10" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>220</v>
+      </c>
+      <c r="C11" t="s">
+        <v>232</v>
+      </c>
+      <c r="D11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>220</v>
+      </c>
+      <c r="C12" t="s">
+        <v>232</v>
+      </c>
+      <c r="D12" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>220</v>
+      </c>
+      <c r="C13" t="s">
+        <v>232</v>
+      </c>
+      <c r="D13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>220</v>
+      </c>
+      <c r="C14" t="s">
+        <v>232</v>
+      </c>
+      <c r="D14" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
+        <v>220</v>
+      </c>
+      <c r="C15" t="s">
+        <v>232</v>
+      </c>
+      <c r="D15" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>220</v>
+      </c>
+      <c r="C16" t="s">
+        <v>232</v>
+      </c>
+      <c r="D16" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>220</v>
+      </c>
+      <c r="C17" t="s">
+        <v>232</v>
+      </c>
+      <c r="D17" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>220</v>
+      </c>
+      <c r="C18" t="s">
+        <v>232</v>
+      </c>
+      <c r="D18" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C19" t="s">
+        <v>232</v>
+      </c>
+      <c r="D19" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" t="s">
+        <v>220</v>
+      </c>
+      <c r="C20" t="s">
+        <v>234</v>
+      </c>
+      <c r="D20" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
+        <v>220</v>
+      </c>
+      <c r="C21" t="s">
+        <v>234</v>
+      </c>
+      <c r="D21" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" t="s">
+        <v>220</v>
+      </c>
+      <c r="C22" t="s">
+        <v>234</v>
+      </c>
+      <c r="D22" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" t="s">
+        <v>220</v>
+      </c>
+      <c r="C23" t="s">
+        <v>234</v>
+      </c>
+      <c r="D23" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" t="s">
+        <v>220</v>
+      </c>
+      <c r="C24" t="s">
+        <v>234</v>
+      </c>
+      <c r="D24" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" t="s">
+        <v>220</v>
+      </c>
+      <c r="C25" t="s">
+        <v>234</v>
+      </c>
+      <c r="D25" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" t="s">
+        <v>220</v>
+      </c>
+      <c r="C26" t="s">
+        <v>234</v>
+      </c>
+      <c r="D26" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C27" t="s">
+        <v>234</v>
+      </c>
+      <c r="D27" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" t="s">
+        <v>220</v>
+      </c>
+      <c r="C28" t="s">
+        <v>234</v>
+      </c>
+      <c r="D28" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" t="s">
+        <v>220</v>
+      </c>
+      <c r="C29" t="s">
+        <v>234</v>
+      </c>
+      <c r="D29" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" t="s">
+        <v>220</v>
+      </c>
+      <c r="C30" t="s">
+        <v>234</v>
+      </c>
+      <c r="D30" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" t="s">
+        <v>220</v>
+      </c>
+      <c r="C31" t="s">
+        <v>234</v>
+      </c>
+      <c r="D31" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" t="s">
+        <v>220</v>
+      </c>
+      <c r="C32" t="s">
+        <v>234</v>
+      </c>
+      <c r="D32" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" t="s">
+        <v>220</v>
+      </c>
+      <c r="C33" t="s">
+        <v>234</v>
+      </c>
+      <c r="D33" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" t="s">
+        <v>220</v>
+      </c>
+      <c r="C34" t="s">
+        <v>234</v>
+      </c>
+      <c r="D34" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" t="s">
+        <v>220</v>
+      </c>
+      <c r="C35" t="s">
+        <v>234</v>
+      </c>
+      <c r="D35" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" t="s">
+        <v>220</v>
+      </c>
+      <c r="C36" t="s">
+        <v>234</v>
+      </c>
+      <c r="D36" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" t="s">
+        <v>220</v>
+      </c>
+      <c r="C37" t="s">
+        <v>234</v>
+      </c>
+      <c r="D37" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" t="s">
+        <v>220</v>
+      </c>
+      <c r="C38" t="s">
+        <v>234</v>
+      </c>
+      <c r="D38" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" t="s">
+        <v>220</v>
+      </c>
+      <c r="C39" t="s">
+        <v>234</v>
+      </c>
+      <c r="D39" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" t="s">
+        <v>220</v>
+      </c>
+      <c r="C40" t="s">
+        <v>234</v>
+      </c>
+      <c r="D40" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" t="s">
+        <v>220</v>
+      </c>
+      <c r="C41" t="s">
+        <v>234</v>
+      </c>
+      <c r="D41" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" t="s">
+        <v>220</v>
+      </c>
+      <c r="C42" t="s">
+        <v>234</v>
+      </c>
+      <c r="D42" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" t="s">
+        <v>220</v>
+      </c>
+      <c r="C43" t="s">
+        <v>234</v>
+      </c>
+      <c r="D43" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" t="s">
+        <v>220</v>
+      </c>
+      <c r="C44" t="s">
+        <v>234</v>
+      </c>
+      <c r="D44" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45" t="s">
+        <v>220</v>
+      </c>
+      <c r="C45" t="s">
+        <v>234</v>
+      </c>
+      <c r="D45" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46" t="s">
+        <v>220</v>
+      </c>
+      <c r="C46" t="s">
+        <v>234</v>
+      </c>
+      <c r="D46" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" t="s">
+        <v>220</v>
+      </c>
+      <c r="C47" t="s">
+        <v>234</v>
+      </c>
+      <c r="D47" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>98</v>
+      </c>
+      <c r="B48" t="s">
+        <v>220</v>
+      </c>
+      <c r="C48" t="s">
+        <v>238</v>
+      </c>
+      <c r="D48" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>99</v>
+      </c>
+      <c r="B49" t="s">
+        <v>220</v>
+      </c>
+      <c r="C49" t="s">
+        <v>238</v>
+      </c>
+      <c r="D49" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50" t="s">
+        <v>220</v>
+      </c>
+      <c r="C50" t="s">
+        <v>238</v>
+      </c>
+      <c r="D50" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>103</v>
+      </c>
+      <c r="B51" t="s">
+        <v>220</v>
+      </c>
+      <c r="C51" t="s">
+        <v>238</v>
+      </c>
+      <c r="D51" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>105</v>
+      </c>
+      <c r="B52" t="s">
+        <v>220</v>
+      </c>
+      <c r="C52" t="s">
+        <v>238</v>
+      </c>
+      <c r="D52" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>107</v>
+      </c>
+      <c r="B53" t="s">
+        <v>220</v>
+      </c>
+      <c r="C53" t="s">
+        <v>238</v>
+      </c>
+      <c r="D53" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>109</v>
+      </c>
+      <c r="B54" t="s">
+        <v>220</v>
+      </c>
+      <c r="C54" t="s">
+        <v>238</v>
+      </c>
+      <c r="D54" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>111</v>
+      </c>
+      <c r="B55" t="s">
+        <v>220</v>
+      </c>
+      <c r="C55" t="s">
+        <v>238</v>
+      </c>
+      <c r="D55" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>113</v>
+      </c>
+      <c r="B56" t="s">
+        <v>220</v>
+      </c>
+      <c r="C56" t="s">
+        <v>238</v>
+      </c>
+      <c r="D56" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>115</v>
+      </c>
+      <c r="B57" t="s">
+        <v>220</v>
+      </c>
+      <c r="C57" t="s">
+        <v>238</v>
+      </c>
+      <c r="D57" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>118</v>
+      </c>
+      <c r="B58" t="s">
+        <v>220</v>
+      </c>
+      <c r="C58" t="s">
+        <v>238</v>
+      </c>
+      <c r="D58" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>119</v>
+      </c>
+      <c r="B59" t="s">
+        <v>220</v>
+      </c>
+      <c r="C59" t="s">
+        <v>238</v>
+      </c>
+      <c r="D59" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>121</v>
+      </c>
+      <c r="B60" t="s">
+        <v>220</v>
+      </c>
+      <c r="C60" t="s">
+        <v>238</v>
+      </c>
+      <c r="D60" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>123</v>
+      </c>
+      <c r="B61" t="s">
+        <v>220</v>
+      </c>
+      <c r="C61" t="s">
+        <v>238</v>
+      </c>
+      <c r="D61" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>125</v>
+      </c>
+      <c r="B62" t="s">
+        <v>220</v>
+      </c>
+      <c r="C62" t="s">
+        <v>238</v>
+      </c>
+      <c r="D62" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>127</v>
+      </c>
+      <c r="B63" t="s">
+        <v>220</v>
+      </c>
+      <c r="C63" t="s">
+        <v>238</v>
+      </c>
+      <c r="D63" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>129</v>
+      </c>
+      <c r="B64" t="s">
+        <v>220</v>
+      </c>
+      <c r="C64" t="s">
+        <v>238</v>
+      </c>
+      <c r="D64" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>131</v>
+      </c>
+      <c r="B65" t="s">
+        <v>220</v>
+      </c>
+      <c r="C65" t="s">
+        <v>238</v>
+      </c>
+      <c r="D65" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>133</v>
+      </c>
+      <c r="B66" t="s">
+        <v>220</v>
+      </c>
+      <c r="C66" t="s">
+        <v>238</v>
+      </c>
+      <c r="D66" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>135</v>
+      </c>
+      <c r="B67" t="s">
+        <v>220</v>
+      </c>
+      <c r="C67" t="s">
+        <v>238</v>
+      </c>
+      <c r="D67" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>137</v>
+      </c>
+      <c r="B68" t="s">
+        <v>220</v>
+      </c>
+      <c r="C68" t="s">
+        <v>238</v>
+      </c>
+      <c r="D68" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>139</v>
+      </c>
+      <c r="B69" t="s">
+        <v>220</v>
+      </c>
+      <c r="C69" t="s">
+        <v>238</v>
+      </c>
+      <c r="D69" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>141</v>
+      </c>
+      <c r="B70" t="s">
+        <v>220</v>
+      </c>
+      <c r="C70" t="s">
+        <v>238</v>
+      </c>
+      <c r="D70" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>143</v>
+      </c>
+      <c r="B71" t="s">
+        <v>220</v>
+      </c>
+      <c r="C71" t="s">
+        <v>238</v>
+      </c>
+      <c r="D71" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>145</v>
+      </c>
+      <c r="B72" t="s">
+        <v>220</v>
+      </c>
+      <c r="C72" t="s">
+        <v>238</v>
+      </c>
+      <c r="D72" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>147</v>
+      </c>
+      <c r="B73" t="s">
+        <v>220</v>
+      </c>
+      <c r="C73" t="s">
+        <v>238</v>
+      </c>
+      <c r="D73" t="s">
+        <v>221</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB85959-D4CA-BD49-876F-6CE6E49A2C93}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
       <c r="B1" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="C1" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="D1" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="E1" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="F1" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="G1" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C2" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="D2" t="s">
-        <v>225</v>
-      </c>
-      <c r="E2" t="s">
-        <v>226</v>
-      </c>
-      <c r="F2" t="s">
-        <v>213</v>
-      </c>
-      <c r="G2" t="s">
-        <v>213</v>
+        <v>231</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>220</v>
       </c>
       <c r="B3" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="C3" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="D3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E3" t="s">
-        <v>226</v>
-      </c>
-      <c r="F3" t="s">
-        <v>213</v>
-      </c>
-      <c r="G3" t="s">
-        <v>213</v>
+        <v>233</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>220</v>
       </c>
       <c r="B4" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
       <c r="C4" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="D4" t="s">
-        <v>225</v>
-      </c>
-      <c r="E4" t="s">
-        <v>226</v>
-      </c>
-      <c r="F4" t="s">
-        <v>213</v>
-      </c>
-      <c r="G4" t="s">
-        <v>213</v>
+        <v>235</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>220</v>
       </c>
       <c r="B5" t="s">
-        <v>223</v>
+        <v>236</v>
       </c>
       <c r="C5" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="D5" t="s">
-        <v>225</v>
-      </c>
-      <c r="E5" t="s">
-        <v>226</v>
-      </c>
-      <c r="F5" t="s">
-        <v>213</v>
-      </c>
-      <c r="G5" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>220</v>
       </c>
       <c r="B6" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="C6" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="D6" t="s">
-        <v>225</v>
-      </c>
-      <c r="E6" t="s">
-        <v>226</v>
-      </c>
-      <c r="F6" t="s">
-        <v>213</v>
-      </c>
-      <c r="G6" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>227</v>
-      </c>
-      <c r="C7" t="s">
-        <v>224</v>
-      </c>
-      <c r="D7" t="s">
-        <v>225</v>
-      </c>
-      <c r="E7" t="s">
-        <v>226</v>
-      </c>
-      <c r="F7" t="s">
-        <v>213</v>
-      </c>
-      <c r="G7" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>223</v>
-      </c>
-      <c r="C8" t="s">
-        <v>224</v>
-      </c>
-      <c r="D8" t="s">
-        <v>225</v>
-      </c>
-      <c r="E8" t="s">
-        <v>226</v>
-      </c>
-      <c r="F8" t="s">
-        <v>213</v>
-      </c>
-      <c r="G8" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>227</v>
-      </c>
-      <c r="C9" t="s">
-        <v>224</v>
-      </c>
-      <c r="D9" t="s">
-        <v>225</v>
-      </c>
-      <c r="E9" t="s">
-        <v>226</v>
-      </c>
-      <c r="F9" t="s">
-        <v>213</v>
-      </c>
-      <c r="G9" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>227</v>
-      </c>
-      <c r="C10" t="s">
-        <v>224</v>
-      </c>
-      <c r="D10" t="s">
-        <v>225</v>
-      </c>
-      <c r="E10" t="s">
-        <v>226</v>
-      </c>
-      <c r="F10" t="s">
-        <v>213</v>
-      </c>
-      <c r="G10" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>227</v>
-      </c>
-      <c r="C11" t="s">
-        <v>224</v>
-      </c>
-      <c r="D11" t="s">
-        <v>225</v>
-      </c>
-      <c r="E11" t="s">
-        <v>226</v>
-      </c>
-      <c r="F11" t="s">
-        <v>213</v>
-      </c>
-      <c r="G11" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" t="s">
-        <v>223</v>
-      </c>
-      <c r="C12" t="s">
-        <v>224</v>
-      </c>
-      <c r="D12" t="s">
-        <v>225</v>
-      </c>
-      <c r="E12" t="s">
-        <v>226</v>
-      </c>
-      <c r="F12" t="s">
-        <v>213</v>
-      </c>
-      <c r="G12" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" t="s">
-        <v>223</v>
-      </c>
-      <c r="C13" t="s">
-        <v>224</v>
-      </c>
-      <c r="D13" t="s">
-        <v>225</v>
-      </c>
-      <c r="E13" t="s">
-        <v>226</v>
-      </c>
-      <c r="F13" t="s">
-        <v>213</v>
-      </c>
-      <c r="G13" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" t="s">
-        <v>228</v>
-      </c>
-      <c r="C14" t="s">
-        <v>224</v>
-      </c>
-      <c r="D14" t="s">
-        <v>225</v>
-      </c>
-      <c r="E14" t="s">
-        <v>226</v>
-      </c>
-      <c r="F14" t="s">
-        <v>229</v>
-      </c>
-      <c r="G14" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" t="s">
-        <v>228</v>
-      </c>
-      <c r="C15" t="s">
-        <v>224</v>
-      </c>
-      <c r="D15" t="s">
-        <v>225</v>
-      </c>
-      <c r="E15" t="s">
-        <v>226</v>
-      </c>
-      <c r="F15" t="s">
-        <v>229</v>
-      </c>
-      <c r="G15" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" t="s">
-        <v>228</v>
-      </c>
-      <c r="C16" t="s">
-        <v>224</v>
-      </c>
-      <c r="D16" t="s">
-        <v>225</v>
-      </c>
-      <c r="E16" t="s">
-        <v>226</v>
-      </c>
-      <c r="F16" t="s">
-        <v>229</v>
-      </c>
-      <c r="G16" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" t="s">
-        <v>228</v>
-      </c>
-      <c r="C17" t="s">
-        <v>224</v>
-      </c>
-      <c r="D17" t="s">
-        <v>225</v>
-      </c>
-      <c r="E17" t="s">
-        <v>226</v>
-      </c>
-      <c r="F17" t="s">
-        <v>229</v>
-      </c>
-      <c r="G17" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" t="s">
-        <v>228</v>
-      </c>
-      <c r="C18" t="s">
-        <v>224</v>
-      </c>
-      <c r="D18" t="s">
-        <v>225</v>
-      </c>
-      <c r="E18" t="s">
-        <v>226</v>
-      </c>
-      <c r="F18" t="s">
-        <v>229</v>
-      </c>
-      <c r="G18" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" t="s">
-        <v>228</v>
-      </c>
-      <c r="C19" t="s">
-        <v>224</v>
-      </c>
-      <c r="D19" t="s">
-        <v>225</v>
-      </c>
-      <c r="E19" t="s">
-        <v>226</v>
-      </c>
-      <c r="F19" t="s">
-        <v>229</v>
-      </c>
-      <c r="G19" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" t="s">
-        <v>230</v>
-      </c>
-      <c r="C20" t="s">
-        <v>224</v>
-      </c>
-      <c r="D20" t="s">
-        <v>225</v>
-      </c>
-      <c r="E20" t="s">
-        <v>226</v>
-      </c>
-      <c r="F20" t="s">
-        <v>213</v>
-      </c>
-      <c r="G20" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" t="s">
-        <v>230</v>
-      </c>
-      <c r="C21" t="s">
-        <v>224</v>
-      </c>
-      <c r="D21" t="s">
-        <v>225</v>
-      </c>
-      <c r="E21" t="s">
-        <v>226</v>
-      </c>
-      <c r="F21" t="s">
-        <v>213</v>
-      </c>
-      <c r="G21" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" t="s">
-        <v>230</v>
-      </c>
-      <c r="C22" t="s">
-        <v>224</v>
-      </c>
-      <c r="D22" t="s">
-        <v>225</v>
-      </c>
-      <c r="E22" t="s">
-        <v>226</v>
-      </c>
-      <c r="F22" t="s">
-        <v>213</v>
-      </c>
-      <c r="G22" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" t="s">
-        <v>230</v>
-      </c>
-      <c r="C23" t="s">
-        <v>224</v>
-      </c>
-      <c r="D23" t="s">
-        <v>225</v>
-      </c>
-      <c r="E23" t="s">
-        <v>226</v>
-      </c>
-      <c r="F23" t="s">
-        <v>213</v>
-      </c>
-      <c r="G23" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" t="s">
-        <v>230</v>
-      </c>
-      <c r="C24" t="s">
-        <v>224</v>
-      </c>
-      <c r="D24" t="s">
-        <v>225</v>
-      </c>
-      <c r="E24" t="s">
-        <v>226</v>
-      </c>
-      <c r="F24" t="s">
-        <v>213</v>
-      </c>
-      <c r="G24" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" t="s">
-        <v>230</v>
-      </c>
-      <c r="C25" t="s">
-        <v>224</v>
-      </c>
-      <c r="D25" t="s">
-        <v>225</v>
-      </c>
-      <c r="E25" t="s">
-        <v>226</v>
-      </c>
-      <c r="F25" t="s">
-        <v>213</v>
-      </c>
-      <c r="G25" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" t="s">
-        <v>230</v>
-      </c>
-      <c r="C26" t="s">
-        <v>224</v>
-      </c>
-      <c r="D26" t="s">
-        <v>225</v>
-      </c>
-      <c r="E26" t="s">
-        <v>226</v>
-      </c>
-      <c r="F26" t="s">
-        <v>213</v>
-      </c>
-      <c r="G26" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" t="s">
-        <v>230</v>
-      </c>
-      <c r="C27" t="s">
-        <v>224</v>
-      </c>
-      <c r="D27" t="s">
-        <v>225</v>
-      </c>
-      <c r="E27" t="s">
-        <v>226</v>
-      </c>
-      <c r="F27" t="s">
-        <v>213</v>
-      </c>
-      <c r="G27" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28" t="s">
-        <v>230</v>
-      </c>
-      <c r="C28" t="s">
-        <v>224</v>
-      </c>
-      <c r="D28" t="s">
-        <v>225</v>
-      </c>
-      <c r="E28" t="s">
-        <v>226</v>
-      </c>
-      <c r="F28" t="s">
-        <v>213</v>
-      </c>
-      <c r="G28" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" t="s">
-        <v>231</v>
-      </c>
-      <c r="C29" t="s">
-        <v>224</v>
-      </c>
-      <c r="D29" t="s">
-        <v>225</v>
-      </c>
-      <c r="E29" t="s">
-        <v>226</v>
-      </c>
-      <c r="F29" t="s">
-        <v>213</v>
-      </c>
-      <c r="G29" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>62</v>
-      </c>
-      <c r="B30" t="s">
-        <v>231</v>
-      </c>
-      <c r="C30" t="s">
-        <v>224</v>
-      </c>
-      <c r="D30" t="s">
-        <v>225</v>
-      </c>
-      <c r="E30" t="s">
-        <v>226</v>
-      </c>
-      <c r="F30" t="s">
-        <v>213</v>
-      </c>
-      <c r="G30" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>64</v>
-      </c>
-      <c r="B31" t="s">
-        <v>231</v>
-      </c>
-      <c r="C31" t="s">
-        <v>224</v>
-      </c>
-      <c r="D31" t="s">
-        <v>225</v>
-      </c>
-      <c r="E31" t="s">
-        <v>226</v>
-      </c>
-      <c r="F31" t="s">
-        <v>213</v>
-      </c>
-      <c r="G31" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>66</v>
-      </c>
-      <c r="B32" t="s">
-        <v>231</v>
-      </c>
-      <c r="C32" t="s">
-        <v>224</v>
-      </c>
-      <c r="D32" t="s">
-        <v>225</v>
-      </c>
-      <c r="E32" t="s">
-        <v>226</v>
-      </c>
-      <c r="F32" t="s">
-        <v>213</v>
-      </c>
-      <c r="G32" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>68</v>
-      </c>
-      <c r="B33" t="s">
-        <v>231</v>
-      </c>
-      <c r="C33" t="s">
-        <v>224</v>
-      </c>
-      <c r="D33" t="s">
-        <v>225</v>
-      </c>
-      <c r="E33" t="s">
-        <v>226</v>
-      </c>
-      <c r="F33" t="s">
-        <v>213</v>
-      </c>
-      <c r="G33" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>70</v>
-      </c>
-      <c r="B34" t="s">
-        <v>231</v>
-      </c>
-      <c r="C34" t="s">
-        <v>224</v>
-      </c>
-      <c r="D34" t="s">
-        <v>225</v>
-      </c>
-      <c r="E34" t="s">
-        <v>226</v>
-      </c>
-      <c r="F34" t="s">
-        <v>213</v>
-      </c>
-      <c r="G34" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>72</v>
-      </c>
-      <c r="B35" t="s">
-        <v>231</v>
-      </c>
-      <c r="C35" t="s">
-        <v>224</v>
-      </c>
-      <c r="D35" t="s">
-        <v>225</v>
-      </c>
-      <c r="E35" t="s">
-        <v>226</v>
-      </c>
-      <c r="F35" t="s">
-        <v>213</v>
-      </c>
-      <c r="G35" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>74</v>
-      </c>
-      <c r="B36" t="s">
-        <v>231</v>
-      </c>
-      <c r="C36" t="s">
-        <v>224</v>
-      </c>
-      <c r="D36" t="s">
-        <v>225</v>
-      </c>
-      <c r="E36" t="s">
-        <v>226</v>
-      </c>
-      <c r="F36" t="s">
-        <v>213</v>
-      </c>
-      <c r="G36" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>76</v>
-      </c>
-      <c r="B37" t="s">
-        <v>231</v>
-      </c>
-      <c r="C37" t="s">
-        <v>224</v>
-      </c>
-      <c r="D37" t="s">
-        <v>225</v>
-      </c>
-      <c r="E37" t="s">
-        <v>226</v>
-      </c>
-      <c r="F37" t="s">
-        <v>213</v>
-      </c>
-      <c r="G37" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>78</v>
-      </c>
-      <c r="B38" t="s">
-        <v>231</v>
-      </c>
-      <c r="C38" t="s">
-        <v>224</v>
-      </c>
-      <c r="D38" t="s">
-        <v>225</v>
-      </c>
-      <c r="E38" t="s">
-        <v>226</v>
-      </c>
-      <c r="F38" t="s">
-        <v>213</v>
-      </c>
-      <c r="G38" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>80</v>
-      </c>
-      <c r="B39" t="s">
-        <v>231</v>
-      </c>
-      <c r="C39" t="s">
-        <v>224</v>
-      </c>
-      <c r="D39" t="s">
-        <v>225</v>
-      </c>
-      <c r="E39" t="s">
-        <v>226</v>
-      </c>
-      <c r="F39" t="s">
-        <v>213</v>
-      </c>
-      <c r="G39" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>82</v>
-      </c>
-      <c r="B40" t="s">
-        <v>231</v>
-      </c>
-      <c r="C40" t="s">
-        <v>224</v>
-      </c>
-      <c r="D40" t="s">
-        <v>225</v>
-      </c>
-      <c r="E40" t="s">
-        <v>226</v>
-      </c>
-      <c r="F40" t="s">
-        <v>213</v>
-      </c>
-      <c r="G40" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>84</v>
-      </c>
-      <c r="B41" t="s">
-        <v>232</v>
-      </c>
-      <c r="C41" t="s">
-        <v>224</v>
-      </c>
-      <c r="D41" t="s">
-        <v>225</v>
-      </c>
-      <c r="E41" t="s">
-        <v>226</v>
-      </c>
-      <c r="F41" t="s">
-        <v>213</v>
-      </c>
-      <c r="G41" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>85</v>
-      </c>
-      <c r="B42" t="s">
-        <v>232</v>
-      </c>
-      <c r="C42" t="s">
-        <v>224</v>
-      </c>
-      <c r="D42" t="s">
-        <v>225</v>
-      </c>
-      <c r="E42" t="s">
-        <v>226</v>
-      </c>
-      <c r="F42" t="s">
-        <v>213</v>
-      </c>
-      <c r="G42" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>87</v>
-      </c>
-      <c r="B43" t="s">
-        <v>232</v>
-      </c>
-      <c r="C43" t="s">
-        <v>224</v>
-      </c>
-      <c r="D43" t="s">
-        <v>225</v>
-      </c>
-      <c r="E43" t="s">
-        <v>226</v>
-      </c>
-      <c r="F43" t="s">
-        <v>213</v>
-      </c>
-      <c r="G43" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>89</v>
-      </c>
-      <c r="B44" t="s">
-        <v>232</v>
-      </c>
-      <c r="C44" t="s">
-        <v>224</v>
-      </c>
-      <c r="D44" t="s">
-        <v>225</v>
-      </c>
-      <c r="E44" t="s">
-        <v>226</v>
-      </c>
-      <c r="F44" t="s">
-        <v>213</v>
-      </c>
-      <c r="G44" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>91</v>
-      </c>
-      <c r="B45" t="s">
-        <v>232</v>
-      </c>
-      <c r="C45" t="s">
-        <v>224</v>
-      </c>
-      <c r="D45" t="s">
-        <v>225</v>
-      </c>
-      <c r="E45" t="s">
-        <v>226</v>
-      </c>
-      <c r="F45" t="s">
-        <v>213</v>
-      </c>
-      <c r="G45" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>93</v>
-      </c>
-      <c r="B46" t="s">
-        <v>232</v>
-      </c>
-      <c r="C46" t="s">
-        <v>224</v>
-      </c>
-      <c r="D46" t="s">
-        <v>225</v>
-      </c>
-      <c r="E46" t="s">
-        <v>226</v>
-      </c>
-      <c r="F46" t="s">
-        <v>213</v>
-      </c>
-      <c r="G46" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>95</v>
-      </c>
-      <c r="B47" t="s">
-        <v>232</v>
-      </c>
-      <c r="C47" t="s">
-        <v>224</v>
-      </c>
-      <c r="D47" t="s">
-        <v>225</v>
-      </c>
-      <c r="E47" t="s">
-        <v>226</v>
-      </c>
-      <c r="F47" t="s">
-        <v>213</v>
-      </c>
-      <c r="G47" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>98</v>
-      </c>
-      <c r="B48" t="s">
-        <v>233</v>
-      </c>
-      <c r="C48" t="s">
-        <v>224</v>
-      </c>
-      <c r="D48" t="s">
-        <v>213</v>
-      </c>
-      <c r="E48" t="s">
-        <v>226</v>
-      </c>
-      <c r="F48" t="s">
-        <v>213</v>
-      </c>
-      <c r="G48" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>99</v>
-      </c>
-      <c r="B49" t="s">
-        <v>233</v>
-      </c>
-      <c r="C49" t="s">
-        <v>224</v>
-      </c>
-      <c r="D49" t="s">
-        <v>213</v>
-      </c>
-      <c r="E49" t="s">
-        <v>226</v>
-      </c>
-      <c r="F49" t="s">
-        <v>213</v>
-      </c>
-      <c r="G49" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>101</v>
-      </c>
-      <c r="B50" t="s">
-        <v>233</v>
-      </c>
-      <c r="C50" t="s">
-        <v>224</v>
-      </c>
-      <c r="D50" t="s">
-        <v>213</v>
-      </c>
-      <c r="E50" t="s">
-        <v>226</v>
-      </c>
-      <c r="F50" t="s">
-        <v>213</v>
-      </c>
-      <c r="G50" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>103</v>
-      </c>
-      <c r="B51" t="s">
-        <v>233</v>
-      </c>
-      <c r="C51" t="s">
-        <v>224</v>
-      </c>
-      <c r="D51" t="s">
-        <v>213</v>
-      </c>
-      <c r="E51" t="s">
-        <v>226</v>
-      </c>
-      <c r="F51" t="s">
-        <v>213</v>
-      </c>
-      <c r="G51" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>105</v>
-      </c>
-      <c r="B52" t="s">
-        <v>233</v>
-      </c>
-      <c r="C52" t="s">
-        <v>224</v>
-      </c>
-      <c r="D52" t="s">
-        <v>213</v>
-      </c>
-      <c r="E52" t="s">
-        <v>226</v>
-      </c>
-      <c r="F52" t="s">
-        <v>213</v>
-      </c>
-      <c r="G52" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>107</v>
-      </c>
-      <c r="B53" t="s">
-        <v>233</v>
-      </c>
-      <c r="C53" t="s">
-        <v>224</v>
-      </c>
-      <c r="D53" t="s">
-        <v>213</v>
-      </c>
-      <c r="E53" t="s">
-        <v>226</v>
-      </c>
-      <c r="F53" t="s">
-        <v>213</v>
-      </c>
-      <c r="G53" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>109</v>
-      </c>
-      <c r="B54" t="s">
-        <v>233</v>
-      </c>
-      <c r="C54" t="s">
-        <v>224</v>
-      </c>
-      <c r="D54" t="s">
-        <v>213</v>
-      </c>
-      <c r="E54" t="s">
-        <v>226</v>
-      </c>
-      <c r="F54" t="s">
-        <v>213</v>
-      </c>
-      <c r="G54" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>111</v>
-      </c>
-      <c r="B55" t="s">
-        <v>233</v>
-      </c>
-      <c r="C55" t="s">
-        <v>224</v>
-      </c>
-      <c r="D55" t="s">
-        <v>213</v>
-      </c>
-      <c r="E55" t="s">
-        <v>226</v>
-      </c>
-      <c r="F55" t="s">
-        <v>213</v>
-      </c>
-      <c r="G55" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>113</v>
-      </c>
-      <c r="B56" t="s">
-        <v>233</v>
-      </c>
-      <c r="C56" t="s">
-        <v>224</v>
-      </c>
-      <c r="D56" t="s">
-        <v>213</v>
-      </c>
-      <c r="E56" t="s">
-        <v>226</v>
-      </c>
-      <c r="F56" t="s">
-        <v>213</v>
-      </c>
-      <c r="G56" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>115</v>
-      </c>
-      <c r="B57" t="s">
-        <v>233</v>
-      </c>
-      <c r="C57" t="s">
-        <v>224</v>
-      </c>
-      <c r="D57" t="s">
-        <v>213</v>
-      </c>
-      <c r="E57" t="s">
-        <v>226</v>
-      </c>
-      <c r="F57" t="s">
-        <v>213</v>
-      </c>
-      <c r="G57" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>118</v>
-      </c>
-      <c r="B58" t="s">
-        <v>234</v>
-      </c>
-      <c r="C58" t="s">
-        <v>224</v>
-      </c>
-      <c r="D58" t="s">
-        <v>213</v>
-      </c>
-      <c r="E58" t="s">
-        <v>226</v>
-      </c>
-      <c r="F58" t="s">
-        <v>213</v>
-      </c>
-      <c r="G58" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>119</v>
-      </c>
-      <c r="B59" t="s">
-        <v>234</v>
-      </c>
-      <c r="C59" t="s">
-        <v>224</v>
-      </c>
-      <c r="D59" t="s">
-        <v>213</v>
-      </c>
-      <c r="E59" t="s">
-        <v>226</v>
-      </c>
-      <c r="F59" t="s">
-        <v>213</v>
-      </c>
-      <c r="G59" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>121</v>
-      </c>
-      <c r="B60" t="s">
-        <v>234</v>
-      </c>
-      <c r="C60" t="s">
-        <v>224</v>
-      </c>
-      <c r="D60" t="s">
-        <v>213</v>
-      </c>
-      <c r="E60" t="s">
-        <v>226</v>
-      </c>
-      <c r="F60" t="s">
-        <v>213</v>
-      </c>
-      <c r="G60" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>123</v>
-      </c>
-      <c r="B61" t="s">
-        <v>234</v>
-      </c>
-      <c r="C61" t="s">
-        <v>224</v>
-      </c>
-      <c r="D61" t="s">
-        <v>213</v>
-      </c>
-      <c r="E61" t="s">
-        <v>226</v>
-      </c>
-      <c r="F61" t="s">
-        <v>213</v>
-      </c>
-      <c r="G61" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>125</v>
-      </c>
-      <c r="B62" t="s">
-        <v>234</v>
-      </c>
-      <c r="C62" t="s">
-        <v>224</v>
-      </c>
-      <c r="D62" t="s">
-        <v>213</v>
-      </c>
-      <c r="E62" t="s">
-        <v>226</v>
-      </c>
-      <c r="F62" t="s">
-        <v>213</v>
-      </c>
-      <c r="G62" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>127</v>
-      </c>
-      <c r="B63" t="s">
-        <v>234</v>
-      </c>
-      <c r="C63" t="s">
-        <v>224</v>
-      </c>
-      <c r="D63" t="s">
-        <v>213</v>
-      </c>
-      <c r="E63" t="s">
-        <v>226</v>
-      </c>
-      <c r="F63" t="s">
-        <v>213</v>
-      </c>
-      <c r="G63" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>129</v>
-      </c>
-      <c r="B64" t="s">
-        <v>234</v>
-      </c>
-      <c r="C64" t="s">
-        <v>224</v>
-      </c>
-      <c r="D64" t="s">
-        <v>213</v>
-      </c>
-      <c r="E64" t="s">
-        <v>226</v>
-      </c>
-      <c r="F64" t="s">
-        <v>213</v>
-      </c>
-      <c r="G64" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>131</v>
-      </c>
-      <c r="B65" t="s">
-        <v>234</v>
-      </c>
-      <c r="C65" t="s">
-        <v>224</v>
-      </c>
-      <c r="D65" t="s">
-        <v>213</v>
-      </c>
-      <c r="E65" t="s">
-        <v>226</v>
-      </c>
-      <c r="F65" t="s">
-        <v>213</v>
-      </c>
-      <c r="G65" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>133</v>
-      </c>
-      <c r="B66" t="s">
-        <v>234</v>
-      </c>
-      <c r="C66" t="s">
-        <v>224</v>
-      </c>
-      <c r="D66" t="s">
-        <v>213</v>
-      </c>
-      <c r="E66" t="s">
-        <v>226</v>
-      </c>
-      <c r="F66" t="s">
-        <v>213</v>
-      </c>
-      <c r="G66" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>135</v>
-      </c>
-      <c r="B67" t="s">
-        <v>234</v>
-      </c>
-      <c r="C67" t="s">
-        <v>224</v>
-      </c>
-      <c r="D67" t="s">
-        <v>213</v>
-      </c>
-      <c r="E67" t="s">
-        <v>226</v>
-      </c>
-      <c r="F67" t="s">
-        <v>213</v>
-      </c>
-      <c r="G67" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>137</v>
-      </c>
-      <c r="B68" t="s">
-        <v>234</v>
-      </c>
-      <c r="C68" t="s">
-        <v>224</v>
-      </c>
-      <c r="D68" t="s">
-        <v>213</v>
-      </c>
-      <c r="E68" t="s">
-        <v>226</v>
-      </c>
-      <c r="F68" t="s">
-        <v>213</v>
-      </c>
-      <c r="G68" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>139</v>
-      </c>
-      <c r="B69" t="s">
-        <v>234</v>
-      </c>
-      <c r="C69" t="s">
-        <v>224</v>
-      </c>
-      <c r="D69" t="s">
-        <v>213</v>
-      </c>
-      <c r="E69" t="s">
-        <v>226</v>
-      </c>
-      <c r="F69" t="s">
-        <v>213</v>
-      </c>
-      <c r="G69" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>141</v>
-      </c>
-      <c r="B70" t="s">
-        <v>234</v>
-      </c>
-      <c r="C70" t="s">
-        <v>224</v>
-      </c>
-      <c r="D70" t="s">
-        <v>213</v>
-      </c>
-      <c r="E70" t="s">
-        <v>226</v>
-      </c>
-      <c r="F70" t="s">
-        <v>213</v>
-      </c>
-      <c r="G70" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>143</v>
-      </c>
-      <c r="B71" t="s">
-        <v>234</v>
-      </c>
-      <c r="C71" t="s">
-        <v>224</v>
-      </c>
-      <c r="D71" t="s">
-        <v>213</v>
-      </c>
-      <c r="E71" t="s">
-        <v>226</v>
-      </c>
-      <c r="F71" t="s">
-        <v>213</v>
-      </c>
-      <c r="G71" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>145</v>
-      </c>
-      <c r="B72" t="s">
-        <v>234</v>
-      </c>
-      <c r="C72" t="s">
-        <v>224</v>
-      </c>
-      <c r="D72" t="s">
-        <v>213</v>
-      </c>
-      <c r="E72" t="s">
-        <v>226</v>
-      </c>
-      <c r="F72" t="s">
-        <v>213</v>
-      </c>
-      <c r="G72" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>147</v>
-      </c>
-      <c r="B73" t="s">
-        <v>234</v>
-      </c>
-      <c r="C73" t="s">
-        <v>224</v>
-      </c>
-      <c r="D73" t="s">
-        <v>213</v>
-      </c>
-      <c r="E73" t="s">
-        <v>226</v>
-      </c>
-      <c r="F73" t="s">
-        <v>213</v>
-      </c>
-      <c r="G73" t="s">
-        <v>213</v>
+        <v>239</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>